<commit_message>
Finished up BOM, changed resistor attributes for zero ohm resistors since they were wrong
</commit_message>
<xml_diff>
--- a/docs/low-gain-radio_BOM.xlsx
+++ b/docs/low-gain-radio_BOM.xlsx
@@ -19,20 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="194">
-  <si>
-    <t>Value</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="189">
   <si>
     <t>MFG</t>
   </si>
   <si>
-    <t>10nF</t>
-  </si>
-  <si>
-    <t>CAPACITOR,</t>
-  </si>
-  <si>
     <t>Digi-Key</t>
   </si>
   <si>
@@ -45,36 +36,24 @@
     <t>GRM188R71H103KA01D</t>
   </si>
   <si>
-    <t>12pF</t>
-  </si>
-  <si>
     <t>490-1405-2-ND</t>
   </si>
   <si>
     <t>GRM1885C1H120JA01D</t>
   </si>
   <si>
-    <t>15pF</t>
-  </si>
-  <si>
     <t>490-1407-2-ND</t>
   </si>
   <si>
     <t>GRM1885C1H150JA01D</t>
   </si>
   <si>
-    <t>2.2pF</t>
-  </si>
-  <si>
     <t>490-9668-2-ND</t>
   </si>
   <si>
     <t>GRM1885C1H2R2CA01D</t>
   </si>
   <si>
-    <t>8.2pF</t>
-  </si>
-  <si>
     <t>06031U8R2BAT2A-ND</t>
   </si>
   <si>
@@ -84,27 +63,18 @@
     <t>06031U8R2BAT2A</t>
   </si>
   <si>
-    <t>10uF</t>
-  </si>
-  <si>
     <t>490-6405-2-ND</t>
   </si>
   <si>
     <t>GRM188R60J106ME47J</t>
   </si>
   <si>
-    <t>100nF</t>
-  </si>
-  <si>
     <t>478-5778-1-ND</t>
   </si>
   <si>
     <t>06035C104JAT2A</t>
   </si>
   <si>
-    <t>1nF</t>
-  </si>
-  <si>
     <t>Digi-key</t>
   </si>
   <si>
@@ -114,18 +84,12 @@
     <t>GRM155R71H102KA01D</t>
   </si>
   <si>
-    <t>6pF</t>
-  </si>
-  <si>
     <t>GQM1875C2E6R0BB12D-ND</t>
   </si>
   <si>
     <t>GQM1875C2E6R0BB12D</t>
   </si>
   <si>
-    <t>1uF</t>
-  </si>
-  <si>
     <t>490-1543-2-ND</t>
   </si>
   <si>
@@ -135,9 +99,6 @@
     <t>C37</t>
   </si>
   <si>
-    <t>2.2uF</t>
-  </si>
-  <si>
     <t>478-3492-2-ND</t>
   </si>
   <si>
@@ -147,12 +108,6 @@
     <t>C43</t>
   </si>
   <si>
-    <t>100uF</t>
-  </si>
-  <si>
-    <t>POLARIZED</t>
-  </si>
-  <si>
     <t>478-1704-1-ND</t>
   </si>
   <si>
@@ -174,33 +129,12 @@
     <t>CF1</t>
   </si>
   <si>
-    <t>ORESAT-CON</t>
-  </si>
-  <si>
-    <t>0-3202045   OreSat 40p</t>
-  </si>
-  <si>
-    <t>M50-3202045.</t>
-  </si>
-  <si>
     <t>CF2</t>
   </si>
   <si>
-    <t>CON-MCX-F-</t>
-  </si>
-  <si>
-    <t>MCX003.062  Linx Techn</t>
-  </si>
-  <si>
     <t>CM1</t>
   </si>
   <si>
-    <t>05+POL+SILK JTAG PIN H</t>
-  </si>
-  <si>
-    <t>standard JTAG connectors. Digi-Key</t>
-  </si>
-  <si>
     <t>1175-1627-ND</t>
   </si>
   <si>
@@ -210,24 +144,12 @@
     <t>3220-10-0100-00</t>
   </si>
   <si>
-    <t>CM2</t>
-  </si>
-  <si>
-    <t>PIN HEADER</t>
-  </si>
-  <si>
-    <t>22nH</t>
-  </si>
-  <si>
     <t>490-6874-1-ND</t>
   </si>
   <si>
     <t>LQW18AN22NG00D</t>
   </si>
   <si>
-    <t>15nH</t>
-  </si>
-  <si>
     <t>490-6866-1-ND</t>
   </si>
   <si>
@@ -237,21 +159,12 @@
     <t>L8</t>
   </si>
   <si>
-    <t>82nH</t>
-  </si>
-  <si>
     <t>490-6912-2-ND</t>
   </si>
   <si>
     <t>LQW18AN82NG00D</t>
   </si>
   <si>
-    <t>GRN</t>
-  </si>
-  <si>
-    <t>Generic LE</t>
-  </si>
-  <si>
     <t>160-1446-1-ND</t>
   </si>
   <si>
@@ -261,12 +174,6 @@
     <t>LTST-C191KGKT</t>
   </si>
   <si>
-    <t>DNP/GRN</t>
-  </si>
-  <si>
-    <t>AMB</t>
-  </si>
-  <si>
     <t>160-1440-1-ND</t>
   </si>
   <si>
@@ -276,9 +183,6 @@
     <t>R1</t>
   </si>
   <si>
-    <t>RESISTOR,</t>
-  </si>
-  <si>
     <t>1276-4592-2-ND</t>
   </si>
   <si>
@@ -288,9 +192,6 @@
     <t>RC1608F2490CS</t>
   </si>
   <si>
-    <t>10k</t>
-  </si>
-  <si>
     <t>311-10.0KHRCT-ND</t>
   </si>
   <si>
@@ -300,42 +201,21 @@
     <t>RC0603FR-0710KL</t>
   </si>
   <si>
-    <t>1k</t>
-  </si>
-  <si>
     <t>311-1.00KHRCT-ND</t>
   </si>
   <si>
     <t>RC0603FR-071KL</t>
   </si>
   <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>DNP/1k</t>
-  </si>
-  <si>
-    <t>R13</t>
-  </si>
-  <si>
-    <t>DNP/0</t>
-  </si>
-  <si>
     <t>SH1</t>
   </si>
   <si>
-    <t>BMI-S-202-</t>
-  </si>
-  <si>
     <t>SH2</t>
   </si>
   <si>
     <t>U1</t>
   </si>
   <si>
-    <t>MKW01Z128</t>
-  </si>
-  <si>
     <t>MKW01Z128CHN-ND</t>
   </si>
   <si>
@@ -348,9 +228,6 @@
     <t>U3</t>
   </si>
   <si>
-    <t>W25Q80DV</t>
-  </si>
-  <si>
     <t>W25Q80DVSSIG-ND</t>
   </si>
   <si>
@@ -366,9 +243,6 @@
     <t>U5</t>
   </si>
   <si>
-    <t>NC7SZ05</t>
-  </si>
-  <si>
     <t>Single Inv</t>
   </si>
   <si>
@@ -381,9 +255,6 @@
     <t>U7</t>
   </si>
   <si>
-    <t>LD39200</t>
-  </si>
-  <si>
     <t>497-15229-2-ND</t>
   </si>
   <si>
@@ -396,9 +267,6 @@
     <t>U9</t>
   </si>
   <si>
-    <t>SKY13405-4</t>
-  </si>
-  <si>
     <t>SKY13405-490LF</t>
   </si>
   <si>
@@ -408,12 +276,6 @@
     <t>Y1</t>
   </si>
   <si>
-    <t>32MHz</t>
-  </si>
-  <si>
-    <t>Crystals</t>
-  </si>
-  <si>
     <t>SER4044CT-ND</t>
   </si>
   <si>
@@ -459,9 +321,6 @@
     <t>Place/Do Not Place (DNP is for final production boards)</t>
   </si>
   <si>
-    <t>Last Modified: 2016.04.14</t>
-  </si>
-  <si>
     <t xml:space="preserve">Generic = </t>
   </si>
   <si>
@@ -489,9 +348,6 @@
     <t xml:space="preserve">Skyworks </t>
   </si>
   <si>
-    <t xml:space="preserve"> MAAL</t>
-  </si>
-  <si>
     <t>MACOM</t>
   </si>
   <si>
@@ -564,21 +420,12 @@
     <t>L3-L6</t>
   </si>
   <si>
-    <t>LED2, LED3</t>
-  </si>
-  <si>
-    <t>LED1, LED4</t>
-  </si>
-  <si>
     <t>LED5-LED8</t>
   </si>
   <si>
     <t>R2, R3, R5</t>
   </si>
   <si>
-    <t>R4, R6, R8-R12, R14</t>
-  </si>
-  <si>
     <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 10uF 6.3Volts 20%</t>
   </si>
   <si>
@@ -601,6 +448,144 @@
   </si>
   <si>
     <t>Fixed Inductors 0603 82nH</t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 50volts 0.1uF 5% X7R</t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 100volts 8.2pF ULTRA LOW ESR</t>
+  </si>
+  <si>
+    <t>Tantalum Capacitors - Solid SMD 10volts 100uF 10%</t>
+  </si>
+  <si>
+    <t>RES SMD 249 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>Thick Film Resistors - SMD 1K OHM 1%</t>
+  </si>
+  <si>
+    <t>Thick Film Resistors - SMD 10K OHM 1%</t>
+  </si>
+  <si>
+    <t>Thick Film Resistors - SMD 1K OHM 1%, DNP</t>
+  </si>
+  <si>
+    <t>Last Modified: 2016.04.27</t>
+  </si>
+  <si>
+    <t>RF Microcontrollers - MCU Kinetis W 32-bit MCU, ARM Cortex-M0+ core, 128KB Flash, 48 MHz, Sub-1GHz Radio, MAPBGA 60</t>
+  </si>
+  <si>
+    <t>RF Amplifier 390-500MHz Gain 35dB 3.6Volt -40C+85C</t>
+  </si>
+  <si>
+    <t>LDO Voltage Regulators 150mA CMOS High Performance LDO</t>
+  </si>
+  <si>
+    <t>RF Amplifier 100-3500MHz 5.5Volt -40C +85C</t>
+  </si>
+  <si>
+    <t>LDO Voltage Regulators Linear Voltage Regulators &amp; Vref</t>
+  </si>
+  <si>
+    <t>Crystals 32MHz 10ppm 12pF -30C +85C</t>
+  </si>
+  <si>
+    <t>RF Switch ICs .01-3GHz SP2T UHL Switch</t>
+  </si>
+  <si>
+    <t>IC FLASH 8MBIT 104MHZ 8SOIC</t>
+  </si>
+  <si>
+    <t>LED GREEN CLEAR 0603 SMD</t>
+  </si>
+  <si>
+    <t>LED AMBER CLEAR 0603 SMD</t>
+  </si>
+  <si>
+    <t>M50-3202045</t>
+  </si>
+  <si>
+    <t>Harwin Inc.</t>
+  </si>
+  <si>
+    <t>952-1381-5-ND</t>
+  </si>
+  <si>
+    <t>Linx Technologies Inc.</t>
+  </si>
+  <si>
+    <t>CONMCX003.062</t>
+  </si>
+  <si>
+    <t>CONMCX003.062-ND</t>
+  </si>
+  <si>
+    <t>10 Positions Header, Shrouded Connector 0.050" (1.27mm) Through Hole Gold</t>
+  </si>
+  <si>
+    <t>CONN MCX JACK 50 OHM EDGE MNT</t>
+  </si>
+  <si>
+    <t>CONN RCPT 1.27MM T/H R/A 40POS</t>
+  </si>
+  <si>
+    <t>CM2/DNP</t>
+  </si>
+  <si>
+    <t>DNP</t>
+  </si>
+  <si>
+    <t>Debug PIN HEADER</t>
+  </si>
+  <si>
+    <t>R4, R8-R12</t>
+  </si>
+  <si>
+    <t>LED1-LED4</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Laird Technologies</t>
+  </si>
+  <si>
+    <t>903-1051-1-ND</t>
+  </si>
+  <si>
+    <t>BMI-S-202-F</t>
+  </si>
+  <si>
+    <t>BMI-S-202-C</t>
+  </si>
+  <si>
+    <t>BOARD SHIELD .65X.65" FRAME</t>
+  </si>
+  <si>
+    <t>BOARD SHIELD .65X.65" COVER</t>
+  </si>
+  <si>
+    <t>903-1014-ND</t>
+  </si>
+  <si>
+    <t>RC0603JR-070RL</t>
+  </si>
+  <si>
+    <t>311-0.0GRTR-ND</t>
+  </si>
+  <si>
+    <t>R6, R7</t>
+  </si>
+  <si>
+    <t>R13, R14</t>
+  </si>
+  <si>
+    <t>Thick Film Resistors - SMD ZERO OHM JUMPER</t>
   </si>
 </sst>
 </file>
@@ -1096,14 +1081,11 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1460,26 +1442,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="V42" sqref="V42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="63.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="82" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="82" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>149</v>
+        <v>102</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1487,10 +1468,9 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1498,38 +1478,35 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>140</v>
+        <v>94</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+      <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1537,255 +1514,249 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>143</v>
+        <v>97</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="C6" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="D6" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>145</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="C7" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="D7" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>148</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H7" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>1</v>
+        <v>89</v>
       </c>
       <c r="E9" t="s">
-        <v>135</v>
+        <v>92</v>
       </c>
       <c r="F9" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="G9" t="s">
-        <v>134</v>
+        <v>86</v>
       </c>
       <c r="H9" t="s">
-        <v>132</v>
+        <v>87</v>
       </c>
       <c r="I9" t="s">
-        <v>133</v>
-      </c>
-      <c r="J9" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>176</v>
+        <v>128</v>
       </c>
       <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>115</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
         <v>2</v>
       </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10" t="s">
-        <v>163</v>
-      </c>
-      <c r="H10" t="s">
-        <v>4</v>
-      </c>
       <c r="I10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>174</v>
+        <v>126</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
       </c>
-      <c r="E11" t="s">
-        <v>10</v>
+      <c r="F11" t="s">
+        <v>116</v>
       </c>
       <c r="G11" t="s">
-        <v>164</v>
+        <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>168</v>
+        <v>120</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" t="s">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>117</v>
       </c>
       <c r="G12" t="s">
-        <v>165</v>
+        <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>167</v>
+        <v>119</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>118</v>
       </c>
       <c r="G13" t="s">
-        <v>166</v>
+        <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" t="s">
-        <v>20</v>
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>144</v>
       </c>
       <c r="G14" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="I14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>172</v>
+        <v>124</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" t="s">
-        <v>23</v>
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>135</v>
       </c>
       <c r="G15" t="s">
-        <v>186</v>
+        <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="I15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>175</v>
+        <v>127</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" t="s">
-        <v>26</v>
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>143</v>
       </c>
       <c r="G16" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="I16" t="s">
-        <v>25</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1793,25 +1764,25 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>170</v>
+        <v>122</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" t="s">
-        <v>30</v>
+        <v>20</v>
+      </c>
+      <c r="F17" t="s">
+        <v>136</v>
       </c>
       <c r="G17" t="s">
-        <v>187</v>
+        <v>18</v>
       </c>
       <c r="H17" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="I17" t="s">
-        <v>29</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1819,25 +1790,25 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>171</v>
+        <v>123</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" t="s">
-        <v>33</v>
+        <v>22</v>
+      </c>
+      <c r="F18" t="s">
+        <v>137</v>
       </c>
       <c r="G18" t="s">
-        <v>188</v>
+        <v>1</v>
       </c>
       <c r="H18" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="I18" t="s">
-        <v>32</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1845,48 +1816,48 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>177</v>
+        <v>129</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" t="s">
-        <v>36</v>
+        <v>24</v>
+      </c>
+      <c r="F19" t="s">
+        <v>138</v>
       </c>
       <c r="G19" t="s">
-        <v>189</v>
+        <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="I19" t="s">
-        <v>35</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>115</v>
+      </c>
+      <c r="G20" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
         <v>2</v>
       </c>
-      <c r="D20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" t="s">
-        <v>163</v>
-      </c>
-      <c r="H20" t="s">
-        <v>4</v>
-      </c>
       <c r="I20" t="s">
-        <v>5</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1894,94 +1865,94 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>178</v>
+        <v>130</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" t="s">
-        <v>40</v>
+        <v>27</v>
+      </c>
+      <c r="F21" t="s">
+        <v>115</v>
       </c>
       <c r="G21" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="I21" t="s">
-        <v>39</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" t="s">
-        <v>45</v>
+        <v>30</v>
+      </c>
+      <c r="F22" t="s">
+        <v>145</v>
       </c>
       <c r="G22" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="I22" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" t="s">
-        <v>48</v>
+        <v>33</v>
+      </c>
+      <c r="F23" t="s">
+        <v>139</v>
       </c>
       <c r="G23" t="s">
-        <v>190</v>
+        <v>18</v>
       </c>
       <c r="H23" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="I23" t="s">
-        <v>47</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" t="s">
-        <v>23</v>
+        <v>15</v>
+      </c>
+      <c r="F24" t="s">
+        <v>135</v>
       </c>
       <c r="G24" t="s">
-        <v>186</v>
+        <v>1</v>
       </c>
       <c r="H24" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="I24" t="s">
-        <v>22</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1989,81 +1960,108 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>173</v>
+        <v>125</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" t="s">
-        <v>30</v>
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>136</v>
       </c>
       <c r="G25" t="s">
-        <v>187</v>
+        <v>18</v>
       </c>
       <c r="H25" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="I25" t="s">
-        <v>29</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>162</v>
+      </c>
+      <c r="D26" t="s">
+        <v>161</v>
+      </c>
+      <c r="F26" t="s">
+        <v>169</v>
       </c>
       <c r="G26" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="H26" t="s">
-        <v>53</v>
+        <v>163</v>
+      </c>
+      <c r="I26" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>164</v>
+      </c>
+      <c r="D27" t="s">
+        <v>165</v>
+      </c>
+      <c r="F27" t="s">
+        <v>168</v>
       </c>
       <c r="G27" t="s">
-        <v>56</v>
-      </c>
-      <c r="H27">
-        <v>3.0619999999999998</v>
+        <v>18</v>
+      </c>
+      <c r="H27" t="s">
+        <v>166</v>
+      </c>
+      <c r="I27" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>57</v>
+        <v>37</v>
+      </c>
+      <c r="C28" t="s">
+        <v>39</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E28" t="s">
-        <v>62</v>
+        <v>40</v>
+      </c>
+      <c r="F28" t="s">
+        <v>167</v>
       </c>
       <c r="G28" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="H28" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="I28" t="s">
-        <v>60</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>63</v>
-      </c>
-      <c r="G29" t="s">
-        <v>64</v>
+        <v>170</v>
+      </c>
+      <c r="E29" t="s">
+        <v>171</v>
+      </c>
+      <c r="F29" t="s">
+        <v>172</v>
+      </c>
+      <c r="I29" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2071,25 +2069,25 @@
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>179</v>
+        <v>131</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" t="s">
-        <v>67</v>
+        <v>42</v>
+      </c>
+      <c r="F30" t="s">
+        <v>140</v>
       </c>
       <c r="G30" t="s">
-        <v>191</v>
+        <v>1</v>
       </c>
       <c r="H30" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="I30" t="s">
-        <v>66</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2097,472 +2095,561 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>180</v>
+        <v>132</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" t="s">
-        <v>70</v>
+        <v>44</v>
+      </c>
+      <c r="F31" t="s">
+        <v>141</v>
       </c>
       <c r="G31" t="s">
-        <v>192</v>
+        <v>1</v>
       </c>
       <c r="H31" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="I31" t="s">
-        <v>69</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>72</v>
+        <v>3</v>
       </c>
       <c r="D32" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" t="s">
-        <v>74</v>
+        <v>47</v>
+      </c>
+      <c r="F32" t="s">
+        <v>142</v>
       </c>
       <c r="G32" t="s">
-        <v>193</v>
+        <v>1</v>
       </c>
       <c r="H32" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="I32" t="s">
-        <v>73</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="D33" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="E33" t="s">
-        <v>79</v>
+        <v>171</v>
+      </c>
+      <c r="F33" t="s">
+        <v>159</v>
       </c>
       <c r="G33" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="H33" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="I33" t="s">
-        <v>77</v>
+        <v>176</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>181</v>
+        <v>133</v>
       </c>
       <c r="C34" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="D34" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="E34" t="s">
-        <v>79</v>
+        <v>171</v>
+      </c>
+      <c r="F34" t="s">
+        <v>160</v>
       </c>
       <c r="G34" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="H34" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="I34" t="s">
-        <v>77</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>4</v>
-      </c>
       <c r="B35" t="s">
-        <v>183</v>
+        <v>53</v>
       </c>
       <c r="C35" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="D35" t="s">
-        <v>78</v>
-      </c>
-      <c r="E35" t="s">
-        <v>83</v>
+        <v>56</v>
+      </c>
+      <c r="F35" t="s">
+        <v>146</v>
       </c>
       <c r="G35" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="H35" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="I35" t="s">
-        <v>82</v>
+        <v>176</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>3</v>
+      </c>
       <c r="B36" t="s">
-        <v>84</v>
-      </c>
-      <c r="C36" s="4">
-        <v>250</v>
+        <v>134</v>
+      </c>
+      <c r="C36" t="s">
+        <v>58</v>
       </c>
       <c r="D36" t="s">
-        <v>87</v>
-      </c>
-      <c r="E36" t="s">
-        <v>88</v>
+        <v>59</v>
+      </c>
+      <c r="F36" t="s">
+        <v>148</v>
       </c>
       <c r="G36" t="s">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="H36" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="I36" t="s">
-        <v>86</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C37" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="D37" t="s">
-        <v>91</v>
-      </c>
-      <c r="E37" t="s">
-        <v>92</v>
+        <v>61</v>
+      </c>
+      <c r="F37" t="s">
+        <v>147</v>
       </c>
       <c r="G37" t="s">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="H37" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="I37" t="s">
-        <v>90</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B38" t="s">
+        <v>186</v>
+      </c>
+      <c r="C38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D38" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" t="s">
+        <v>171</v>
+      </c>
+      <c r="F38" t="s">
+        <v>149</v>
+      </c>
+      <c r="G38" t="s">
+        <v>1</v>
+      </c>
+      <c r="H38" t="s">
+        <v>60</v>
+      </c>
+      <c r="I38" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>187</v>
+      </c>
+      <c r="C39" t="s">
+        <v>58</v>
+      </c>
+      <c r="D39" t="s">
+        <v>184</v>
+      </c>
+      <c r="E39" t="s">
+        <v>171</v>
+      </c>
+      <c r="F39" t="s">
+        <v>188</v>
+      </c>
+      <c r="G39" t="s">
+        <v>1</v>
+      </c>
+      <c r="H39" t="s">
         <v>185</v>
       </c>
-      <c r="C38" t="s">
-        <v>93</v>
-      </c>
-      <c r="D38" t="s">
-        <v>91</v>
-      </c>
-      <c r="E38" t="s">
-        <v>95</v>
-      </c>
-      <c r="G38" t="s">
-        <v>85</v>
-      </c>
-      <c r="H38" t="s">
-        <v>4</v>
-      </c>
-      <c r="I38" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>96</v>
-      </c>
-      <c r="C39" t="s">
-        <v>97</v>
-      </c>
-      <c r="D39" t="s">
-        <v>91</v>
-      </c>
-      <c r="E39" t="s">
-        <v>95</v>
-      </c>
-      <c r="G39" t="s">
-        <v>85</v>
-      </c>
-      <c r="H39" t="s">
-        <v>4</v>
-      </c>
       <c r="I39" t="s">
-        <v>94</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="C40" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D40" t="s">
-        <v>91</v>
-      </c>
-      <c r="E40" t="s">
-        <v>95</v>
+        <v>110</v>
+      </c>
+      <c r="F40" t="s">
+        <v>151</v>
       </c>
       <c r="G40" t="s">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="H40" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="I40" t="s">
-        <v>94</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="C41" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D41" t="s">
-        <v>150</v>
-      </c>
-      <c r="E41" t="s">
-        <v>158</v>
+        <v>67</v>
+      </c>
+      <c r="F41" t="s">
+        <v>152</v>
+      </c>
+      <c r="G41" t="s">
+        <v>72</v>
       </c>
       <c r="H41" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="I41" t="s">
-        <v>105</v>
+        <v>175</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>106</v>
+        <v>68</v>
       </c>
       <c r="C42" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D42" t="s">
-        <v>155</v>
-      </c>
-      <c r="E42" t="s">
-        <v>107</v>
+        <v>105</v>
+      </c>
+      <c r="F42" t="s">
+        <v>158</v>
+      </c>
+      <c r="G42" t="s">
+        <v>1</v>
       </c>
       <c r="H42" t="s">
-        <v>113</v>
+        <v>69</v>
       </c>
       <c r="I42" t="s">
-        <v>107</v>
+        <v>176</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" t="s">
         <v>108</v>
       </c>
-      <c r="C43" t="s">
-        <v>109</v>
-      </c>
       <c r="D43" t="s">
-        <v>151</v>
-      </c>
-      <c r="E43" t="s">
-        <v>152</v>
+        <v>71</v>
+      </c>
+      <c r="F43" t="s">
+        <v>153</v>
+      </c>
+      <c r="G43" t="s">
+        <v>72</v>
       </c>
       <c r="H43" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="I43" t="s">
-        <v>110</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>111</v>
+        <v>73</v>
       </c>
       <c r="C44" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D44" t="s">
-        <v>155</v>
-      </c>
-      <c r="E44" t="s">
-        <v>112</v>
+        <v>107</v>
+      </c>
+      <c r="F44" t="s">
+        <v>74</v>
+      </c>
+      <c r="G44" t="s">
+        <v>1</v>
       </c>
       <c r="H44" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="I44" t="s">
-        <v>112</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="C45" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D45" t="s">
+        <v>71</v>
+      </c>
+      <c r="F45" t="s">
         <v>153</v>
       </c>
-      <c r="E45" t="s">
-        <v>154</v>
-      </c>
       <c r="G45" t="s">
-        <v>116</v>
+        <v>72</v>
       </c>
       <c r="H45" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="I45" t="s">
-        <v>117</v>
+        <v>176</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>118</v>
+        <v>77</v>
       </c>
       <c r="C46" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
       <c r="D46" t="s">
+        <v>111</v>
+      </c>
+      <c r="F46" t="s">
         <v>155</v>
       </c>
-      <c r="E46" t="s">
-        <v>112</v>
+      <c r="G46" t="s">
+        <v>1</v>
       </c>
       <c r="H46" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="I46" t="s">
-        <v>112</v>
+        <v>176</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>119</v>
+        <v>80</v>
       </c>
       <c r="C47" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="D47" t="s">
-        <v>122</v>
-      </c>
-      <c r="E47" t="s">
-        <v>159</v>
+        <v>112</v>
+      </c>
+      <c r="F47" t="s">
+        <v>154</v>
+      </c>
+      <c r="G47" t="s">
+        <v>109</v>
       </c>
       <c r="H47" t="s">
-        <v>4</v>
+        <v>112</v>
       </c>
       <c r="I47" t="s">
-        <v>121</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>123</v>
+        <v>81</v>
       </c>
       <c r="C48" t="s">
-        <v>160</v>
+        <v>108</v>
       </c>
       <c r="D48" t="s">
+        <v>82</v>
+      </c>
+      <c r="F48" t="s">
         <v>157</v>
       </c>
-      <c r="E48" t="s">
-        <v>160</v>
-      </c>
       <c r="G48" t="s">
-        <v>156</v>
+        <v>1</v>
       </c>
       <c r="H48" t="s">
-        <v>157</v>
+        <v>83</v>
       </c>
       <c r="I48" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>124</v>
+        <v>84</v>
       </c>
       <c r="C49" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="D49" t="s">
-        <v>155</v>
-      </c>
-      <c r="E49" t="s">
-        <v>126</v>
+        <v>114</v>
+      </c>
+      <c r="F49" t="s">
+        <v>156</v>
+      </c>
+      <c r="G49" t="s">
+        <v>1</v>
       </c>
       <c r="H49" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="I49" t="s">
-        <v>127</v>
+        <v>176</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>128</v>
+        <v>62</v>
       </c>
       <c r="C50" t="s">
-        <v>129</v>
+        <v>177</v>
       </c>
       <c r="D50" t="s">
-        <v>161</v>
-      </c>
-      <c r="E50" t="s">
-        <v>162</v>
+        <v>180</v>
+      </c>
+      <c r="F50" t="s">
+        <v>182</v>
       </c>
       <c r="G50" t="s">
-        <v>130</v>
+        <v>1</v>
       </c>
       <c r="H50" t="s">
-        <v>4</v>
+        <v>183</v>
       </c>
       <c r="I50" t="s">
-        <v>131</v>
+        <v>175</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>100</v>
+        <v>62</v>
       </c>
       <c r="C51" t="s">
-        <v>101</v>
+        <v>177</v>
+      </c>
+      <c r="D51" t="s">
+        <v>179</v>
+      </c>
+      <c r="F51" t="s">
+        <v>181</v>
+      </c>
+      <c r="G51" t="s">
+        <v>1</v>
+      </c>
+      <c r="H51" t="s">
+        <v>178</v>
+      </c>
+      <c r="I51" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="C52" t="s">
-        <v>101</v>
+        <v>177</v>
+      </c>
+      <c r="D52" t="s">
+        <v>180</v>
+      </c>
+      <c r="F52" t="s">
+        <v>182</v>
+      </c>
+      <c r="G52" t="s">
+        <v>1</v>
+      </c>
+      <c r="H52" t="s">
+        <v>183</v>
+      </c>
+      <c r="I52" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" t="s">
+        <v>177</v>
+      </c>
+      <c r="D53" t="s">
+        <v>179</v>
+      </c>
+      <c r="F53" t="s">
+        <v>181</v>
+      </c>
+      <c r="G53" t="s">
+        <v>1</v>
+      </c>
+      <c r="H53" t="s">
+        <v>178</v>
+      </c>
+      <c r="I53" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed some definitions, vendors and vendor PNs
</commit_message>
<xml_diff>
--- a/docs/low-gain-radio_BOM.xlsx
+++ b/docs/low-gain-radio_BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="192">
   <si>
     <t>MFG</t>
   </si>
@@ -237,9 +237,6 @@
     <t>AAT3215</t>
   </si>
   <si>
-    <t>Skyworks</t>
-  </si>
-  <si>
     <t>U5</t>
   </si>
   <si>
@@ -586,6 +583,18 @@
   </si>
   <si>
     <t>Thick Film Resistors - SMD ZERO OHM JUMPER</t>
+  </si>
+  <si>
+    <t>1465-1261-1-ND</t>
+  </si>
+  <si>
+    <t>873-AAT3215IGV-30T1</t>
+  </si>
+  <si>
+    <t>873-SKY65116-21</t>
+  </si>
+  <si>
+    <t>Mouser</t>
   </si>
 </sst>
 </file>
@@ -1445,7 +1454,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="V42" sqref="V42"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1455,12 +1464,13 @@
     <col min="4" max="4" width="63.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="82" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1482,7 +1492,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="1"/>
@@ -1494,7 +1504,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="1"/>
@@ -1506,7 +1516,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1518,14 +1528,14 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -1534,14 +1544,14 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -1550,31 +1560,31 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" t="s">
         <v>90</v>
-      </c>
-      <c r="B9" t="s">
-        <v>91</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I9" t="s">
         <v>92</v>
-      </c>
-      <c r="F9" t="s">
-        <v>88</v>
-      </c>
-      <c r="G9" t="s">
-        <v>86</v>
-      </c>
-      <c r="H9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I9" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1582,7 +1592,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
@@ -1591,7 +1601,7 @@
         <v>4</v>
       </c>
       <c r="F10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G10" t="s">
         <v>1</v>
@@ -1600,7 +1610,7 @@
         <v>2</v>
       </c>
       <c r="I10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1608,7 +1618,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
@@ -1617,7 +1627,7 @@
         <v>6</v>
       </c>
       <c r="F11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G11" t="s">
         <v>1</v>
@@ -1626,7 +1636,7 @@
         <v>5</v>
       </c>
       <c r="I11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1634,7 +1644,7 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
@@ -1643,7 +1653,7 @@
         <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G12" t="s">
         <v>1</v>
@@ -1652,7 +1662,7 @@
         <v>7</v>
       </c>
       <c r="I12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1660,7 +1670,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
@@ -1669,7 +1679,7 @@
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G13" t="s">
         <v>1</v>
@@ -1678,7 +1688,7 @@
         <v>9</v>
       </c>
       <c r="I13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1686,7 +1696,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -1695,7 +1705,7 @@
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G14" t="s">
         <v>1</v>
@@ -1704,7 +1714,7 @@
         <v>11</v>
       </c>
       <c r="I14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1712,7 +1722,7 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -1721,7 +1731,7 @@
         <v>15</v>
       </c>
       <c r="F15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G15" t="s">
         <v>1</v>
@@ -1730,7 +1740,7 @@
         <v>14</v>
       </c>
       <c r="I15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1738,7 +1748,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
@@ -1747,7 +1757,7 @@
         <v>17</v>
       </c>
       <c r="F16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G16" t="s">
         <v>1</v>
@@ -1756,7 +1766,7 @@
         <v>16</v>
       </c>
       <c r="I16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1764,7 +1774,7 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
@@ -1773,7 +1783,7 @@
         <v>20</v>
       </c>
       <c r="F17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G17" t="s">
         <v>18</v>
@@ -1782,7 +1792,7 @@
         <v>19</v>
       </c>
       <c r="I17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1790,7 +1800,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
@@ -1799,7 +1809,7 @@
         <v>22</v>
       </c>
       <c r="F18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G18" t="s">
         <v>1</v>
@@ -1808,7 +1818,7 @@
         <v>21</v>
       </c>
       <c r="I18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1816,7 +1826,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C19" t="s">
         <v>3</v>
@@ -1825,7 +1835,7 @@
         <v>24</v>
       </c>
       <c r="F19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G19" t="s">
         <v>1</v>
@@ -1834,7 +1844,7 @@
         <v>23</v>
       </c>
       <c r="I19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1848,7 +1858,7 @@
         <v>4</v>
       </c>
       <c r="F20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G20" t="s">
         <v>1</v>
@@ -1857,7 +1867,7 @@
         <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1865,7 +1875,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C21" t="s">
         <v>12</v>
@@ -1874,7 +1884,7 @@
         <v>27</v>
       </c>
       <c r="F21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G21" t="s">
         <v>1</v>
@@ -1883,7 +1893,7 @@
         <v>26</v>
       </c>
       <c r="I21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1897,7 +1907,7 @@
         <v>30</v>
       </c>
       <c r="F22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G22" t="s">
         <v>1</v>
@@ -1906,7 +1916,7 @@
         <v>29</v>
       </c>
       <c r="I22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1920,7 +1930,7 @@
         <v>33</v>
       </c>
       <c r="F23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G23" t="s">
         <v>18</v>
@@ -1929,7 +1939,7 @@
         <v>32</v>
       </c>
       <c r="I23" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1943,7 +1953,7 @@
         <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G24" t="s">
         <v>1</v>
@@ -1952,7 +1962,7 @@
         <v>14</v>
       </c>
       <c r="I24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1960,7 +1970,7 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C25" t="s">
         <v>3</v>
@@ -1969,7 +1979,7 @@
         <v>20</v>
       </c>
       <c r="F25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G25" t="s">
         <v>18</v>
@@ -1978,7 +1988,7 @@
         <v>19</v>
       </c>
       <c r="I25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1986,22 +1996,22 @@
         <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D26" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G26" t="s">
         <v>18</v>
       </c>
       <c r="H26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I26" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -2009,22 +2019,22 @@
         <v>36</v>
       </c>
       <c r="C27" t="s">
+        <v>163</v>
+      </c>
+      <c r="D27" t="s">
         <v>164</v>
       </c>
-      <c r="D27" t="s">
-        <v>165</v>
-      </c>
       <c r="F27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G27" t="s">
         <v>18</v>
       </c>
       <c r="H27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -2038,7 +2048,7 @@
         <v>40</v>
       </c>
       <c r="F28" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G28" t="s">
         <v>18</v>
@@ -2047,21 +2057,21 @@
         <v>38</v>
       </c>
       <c r="I28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>169</v>
+      </c>
+      <c r="E29" t="s">
         <v>170</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>171</v>
       </c>
-      <c r="F29" t="s">
-        <v>172</v>
-      </c>
       <c r="I29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2069,7 +2079,7 @@
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C30" t="s">
         <v>3</v>
@@ -2078,7 +2088,7 @@
         <v>42</v>
       </c>
       <c r="F30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G30" t="s">
         <v>1</v>
@@ -2087,7 +2097,7 @@
         <v>41</v>
       </c>
       <c r="I30" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2095,7 +2105,7 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C31" t="s">
         <v>3</v>
@@ -2104,7 +2114,7 @@
         <v>44</v>
       </c>
       <c r="F31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G31" t="s">
         <v>1</v>
@@ -2113,7 +2123,7 @@
         <v>43</v>
       </c>
       <c r="I31" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2127,7 +2137,7 @@
         <v>47</v>
       </c>
       <c r="F32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G32" t="s">
         <v>1</v>
@@ -2136,7 +2146,7 @@
         <v>46</v>
       </c>
       <c r="I32" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2144,7 +2154,7 @@
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C33" t="s">
         <v>49</v>
@@ -2153,10 +2163,10 @@
         <v>50</v>
       </c>
       <c r="E33" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G33" t="s">
         <v>1</v>
@@ -2165,7 +2175,7 @@
         <v>48</v>
       </c>
       <c r="I33" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2173,7 +2183,7 @@
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C34" t="s">
         <v>49</v>
@@ -2182,10 +2192,10 @@
         <v>52</v>
       </c>
       <c r="E34" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G34" t="s">
         <v>1</v>
@@ -2194,7 +2204,7 @@
         <v>51</v>
       </c>
       <c r="I34" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2208,7 +2218,7 @@
         <v>56</v>
       </c>
       <c r="F35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G35" t="s">
         <v>1</v>
@@ -2217,7 +2227,7 @@
         <v>54</v>
       </c>
       <c r="I35" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -2225,7 +2235,7 @@
         <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C36" t="s">
         <v>58</v>
@@ -2234,7 +2244,7 @@
         <v>59</v>
       </c>
       <c r="F36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G36" t="s">
         <v>1</v>
@@ -2243,7 +2253,7 @@
         <v>57</v>
       </c>
       <c r="I36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2251,7 +2261,7 @@
         <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C37" t="s">
         <v>58</v>
@@ -2260,7 +2270,7 @@
         <v>61</v>
       </c>
       <c r="F37" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G37" t="s">
         <v>1</v>
@@ -2269,7 +2279,7 @@
         <v>60</v>
       </c>
       <c r="I37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2277,7 +2287,7 @@
         <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C38" t="s">
         <v>58</v>
@@ -2286,10 +2296,10 @@
         <v>61</v>
       </c>
       <c r="E38" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G38" t="s">
         <v>1</v>
@@ -2298,7 +2308,7 @@
         <v>60</v>
       </c>
       <c r="I38" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2306,28 +2316,28 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C39" t="s">
         <v>58</v>
       </c>
       <c r="D39" t="s">
+        <v>183</v>
+      </c>
+      <c r="E39" t="s">
+        <v>170</v>
+      </c>
+      <c r="F39" t="s">
+        <v>187</v>
+      </c>
+      <c r="G39" t="s">
+        <v>1</v>
+      </c>
+      <c r="H39" t="s">
         <v>184</v>
       </c>
-      <c r="E39" t="s">
-        <v>171</v>
-      </c>
-      <c r="F39" t="s">
-        <v>188</v>
-      </c>
-      <c r="G39" t="s">
-        <v>1</v>
-      </c>
-      <c r="H39" t="s">
-        <v>185</v>
-      </c>
       <c r="I39" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2335,13 +2345,13 @@
         <v>64</v>
       </c>
       <c r="C40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F40" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G40" t="s">
         <v>1</v>
@@ -2350,7 +2360,7 @@
         <v>65</v>
       </c>
       <c r="I40" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2358,22 +2368,22 @@
         <v>66</v>
       </c>
       <c r="C41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D41" t="s">
         <v>67</v>
       </c>
       <c r="F41" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G41" t="s">
-        <v>72</v>
+        <v>191</v>
       </c>
       <c r="H41" t="s">
-        <v>67</v>
+        <v>190</v>
       </c>
       <c r="I41" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2381,13 +2391,13 @@
         <v>68</v>
       </c>
       <c r="C42" t="s">
+        <v>103</v>
+      </c>
+      <c r="D42" t="s">
         <v>104</v>
       </c>
-      <c r="D42" t="s">
-        <v>105</v>
-      </c>
       <c r="F42" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G42" t="s">
         <v>1</v>
@@ -2396,7 +2406,7 @@
         <v>69</v>
       </c>
       <c r="I42" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2404,160 +2414,160 @@
         <v>70</v>
       </c>
       <c r="C43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D43" t="s">
         <v>71</v>
       </c>
       <c r="F43" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G43" t="s">
-        <v>72</v>
+        <v>191</v>
       </c>
       <c r="H43" t="s">
-        <v>71</v>
+        <v>189</v>
       </c>
       <c r="I43" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" t="s">
+        <v>105</v>
+      </c>
+      <c r="D44" t="s">
+        <v>106</v>
+      </c>
+      <c r="F44" t="s">
         <v>73</v>
       </c>
-      <c r="C44" t="s">
-        <v>106</v>
-      </c>
-      <c r="D44" t="s">
-        <v>107</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
+        <v>1</v>
+      </c>
+      <c r="H44" t="s">
         <v>74</v>
       </c>
-      <c r="G44" t="s">
-        <v>1</v>
-      </c>
-      <c r="H44" t="s">
-        <v>75</v>
-      </c>
       <c r="I44" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C45" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D45" t="s">
         <v>71</v>
       </c>
       <c r="F45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G45" t="s">
-        <v>72</v>
+        <v>191</v>
       </c>
       <c r="H45" t="s">
-        <v>71</v>
+        <v>189</v>
       </c>
       <c r="I45" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" t="s">
+        <v>110</v>
+      </c>
+      <c r="F46" t="s">
+        <v>154</v>
+      </c>
+      <c r="G46" t="s">
+        <v>1</v>
+      </c>
+      <c r="H46" t="s">
         <v>77</v>
       </c>
-      <c r="C46" t="s">
-        <v>79</v>
-      </c>
-      <c r="D46" t="s">
-        <v>111</v>
-      </c>
-      <c r="F46" t="s">
-        <v>155</v>
-      </c>
-      <c r="G46" t="s">
-        <v>1</v>
-      </c>
-      <c r="H46" t="s">
-        <v>78</v>
-      </c>
       <c r="I46" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C47" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D47" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G47" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="H47" t="s">
-        <v>112</v>
+        <v>188</v>
       </c>
       <c r="I47" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
+        <v>80</v>
+      </c>
+      <c r="C48" t="s">
+        <v>107</v>
+      </c>
+      <c r="D48" t="s">
         <v>81</v>
       </c>
-      <c r="C48" t="s">
-        <v>108</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="F48" t="s">
+        <v>156</v>
+      </c>
+      <c r="G48" t="s">
+        <v>1</v>
+      </c>
+      <c r="H48" t="s">
         <v>82</v>
       </c>
-      <c r="F48" t="s">
-        <v>157</v>
-      </c>
-      <c r="G48" t="s">
-        <v>1</v>
-      </c>
-      <c r="H48" t="s">
-        <v>83</v>
-      </c>
       <c r="I48" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" t="s">
+        <v>112</v>
+      </c>
+      <c r="D49" t="s">
+        <v>113</v>
+      </c>
+      <c r="F49" t="s">
+        <v>155</v>
+      </c>
+      <c r="G49" t="s">
+        <v>1</v>
+      </c>
+      <c r="H49" t="s">
         <v>84</v>
       </c>
-      <c r="C49" t="s">
-        <v>113</v>
-      </c>
-      <c r="D49" t="s">
-        <v>114</v>
-      </c>
-      <c r="F49" t="s">
-        <v>156</v>
-      </c>
-      <c r="G49" t="s">
-        <v>1</v>
-      </c>
-      <c r="H49" t="s">
-        <v>85</v>
-      </c>
       <c r="I49" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
@@ -2565,22 +2575,22 @@
         <v>62</v>
       </c>
       <c r="C50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D50" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F50" t="s">
+        <v>181</v>
+      </c>
+      <c r="G50" t="s">
+        <v>1</v>
+      </c>
+      <c r="H50" t="s">
         <v>182</v>
       </c>
-      <c r="G50" t="s">
-        <v>1</v>
-      </c>
-      <c r="H50" t="s">
-        <v>183</v>
-      </c>
       <c r="I50" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
@@ -2588,22 +2598,22 @@
         <v>62</v>
       </c>
       <c r="C51" t="s">
+        <v>176</v>
+      </c>
+      <c r="D51" t="s">
+        <v>178</v>
+      </c>
+      <c r="F51" t="s">
+        <v>180</v>
+      </c>
+      <c r="G51" t="s">
+        <v>1</v>
+      </c>
+      <c r="H51" t="s">
         <v>177</v>
       </c>
-      <c r="D51" t="s">
-        <v>179</v>
-      </c>
-      <c r="F51" t="s">
-        <v>181</v>
-      </c>
-      <c r="G51" t="s">
-        <v>1</v>
-      </c>
-      <c r="H51" t="s">
-        <v>178</v>
-      </c>
       <c r="I51" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
@@ -2611,22 +2621,22 @@
         <v>63</v>
       </c>
       <c r="C52" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D52" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F52" t="s">
+        <v>181</v>
+      </c>
+      <c r="G52" t="s">
+        <v>1</v>
+      </c>
+      <c r="H52" t="s">
         <v>182</v>
       </c>
-      <c r="G52" t="s">
-        <v>1</v>
-      </c>
-      <c r="H52" t="s">
-        <v>183</v>
-      </c>
       <c r="I52" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
@@ -2634,22 +2644,22 @@
         <v>63</v>
       </c>
       <c r="C53" t="s">
+        <v>176</v>
+      </c>
+      <c r="D53" t="s">
+        <v>178</v>
+      </c>
+      <c r="F53" t="s">
+        <v>180</v>
+      </c>
+      <c r="G53" t="s">
+        <v>1</v>
+      </c>
+      <c r="H53" t="s">
         <v>177</v>
       </c>
-      <c r="D53" t="s">
-        <v>179</v>
-      </c>
-      <c r="F53" t="s">
-        <v>181</v>
-      </c>
-      <c r="G53" t="s">
-        <v>1</v>
-      </c>
-      <c r="H53" t="s">
-        <v>178</v>
-      </c>
       <c r="I53" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced old with new LDOs in the BOM
</commit_message>
<xml_diff>
--- a/docs/low-gain-radio_BOM.xlsx
+++ b/docs/low-gain-radio_BOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -183,9 +183,6 @@
     <t>U4</t>
   </si>
   <si>
-    <t>AAT3215</t>
-  </si>
-  <si>
     <t>U5</t>
   </si>
   <si>
@@ -399,9 +396,6 @@
     <t>RF Amplifier 390-500MHz Gain 35dB 3.6Volt -40C+85C</t>
   </si>
   <si>
-    <t>LDO Voltage Regulators 150mA CMOS High Performance LDO</t>
-  </si>
-  <si>
     <t>RF Amplifier 100-3500MHz 5.5Volt -40C +85C</t>
   </si>
   <si>
@@ -525,12 +519,6 @@
     <t>581-06031U8R2BAT2A</t>
   </si>
   <si>
-    <t>AAT3215IGV-3.0-T1</t>
-  </si>
-  <si>
-    <t>Skyworks</t>
-  </si>
-  <si>
     <t>GQM1885C2A6R0CB01D</t>
   </si>
   <si>
@@ -583,13 +571,25 @@
   </si>
   <si>
     <t>IC INVERTER UHS OPEN DRN SC70-5</t>
+  </si>
+  <si>
+    <t>LP5907MFX-3.3</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>IC REG LDO 3.3V 0.25A SOT23-5</t>
+  </si>
+  <si>
+    <t>296-38557-1-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -734,6 +734,13 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Sans"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1078,12 +1085,15 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1442,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1461,7 +1471,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1483,7 +1493,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4"/>
@@ -1495,7 +1505,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="4"/>
@@ -1507,7 +1517,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1519,14 +1529,14 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -1535,14 +1545,14 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1551,31 +1561,31 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1583,7 +1593,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>2</v>
@@ -1592,16 +1602,16 @@
         <v>3</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1609,7 +1619,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>2</v>
@@ -1618,16 +1628,16 @@
         <v>4</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1635,7 +1645,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>2</v>
@@ -1644,16 +1654,16 @@
         <v>5</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1661,7 +1671,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>2</v>
@@ -1670,16 +1680,16 @@
         <v>6</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1687,7 +1697,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>7</v>
@@ -1696,16 +1706,16 @@
         <v>8</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1713,7 +1723,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>2</v>
@@ -1722,16 +1732,16 @@
         <v>9</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1739,7 +1749,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>7</v>
@@ -1748,7 +1758,7 @@
         <v>11</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>1</v>
@@ -1757,7 +1767,7 @@
         <v>10</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1765,7 +1775,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>2</v>
@@ -1774,7 +1784,7 @@
         <v>14</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>12</v>
@@ -1783,7 +1793,7 @@
         <v>13</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1791,25 +1801,25 @@
         <v>2</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1817,7 +1827,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>2</v>
@@ -1826,16 +1836,16 @@
         <v>15</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1849,7 +1859,7 @@
         <v>18</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>1</v>
@@ -1858,7 +1868,7 @@
         <v>17</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1872,7 +1882,7 @@
         <v>21</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>12</v>
@@ -1881,7 +1891,7 @@
         <v>20</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1889,7 +1899,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>2</v>
@@ -1898,7 +1908,7 @@
         <v>14</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>12</v>
@@ -1907,7 +1917,7 @@
         <v>13</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1915,22 +1925,22 @@
         <v>22</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1938,22 +1948,22 @@
         <v>23</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D24" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>140</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1967,7 +1977,7 @@
         <v>27</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>12</v>
@@ -1976,21 +1986,21 @@
         <v>25</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="B26" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>144</v>
-      </c>
       <c r="I26" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1998,7 +2008,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>2</v>
@@ -2007,7 +2017,7 @@
         <v>29</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>1</v>
@@ -2016,7 +2026,7 @@
         <v>28</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -2024,7 +2034,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>2</v>
@@ -2033,7 +2043,7 @@
         <v>31</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>1</v>
@@ -2042,7 +2052,7 @@
         <v>30</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -2056,16 +2066,16 @@
         <v>33</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -2073,7 +2083,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>35</v>
@@ -2082,10 +2092,10 @@
         <v>36</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>1</v>
@@ -2094,7 +2104,7 @@
         <v>34</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -2102,28 +2112,28 @@
         <v>4</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -2137,16 +2147,16 @@
         <v>39</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -2154,7 +2164,7 @@
         <v>3</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>41</v>
@@ -2163,7 +2173,7 @@
         <v>42</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>1</v>
@@ -2172,7 +2182,7 @@
         <v>40</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -2180,7 +2190,7 @@
         <v>6</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>41</v>
@@ -2189,7 +2199,7 @@
         <v>44</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>1</v>
@@ -2198,7 +2208,7 @@
         <v>43</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -2206,7 +2216,7 @@
         <v>2</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>41</v>
@@ -2215,10 +2225,10 @@
         <v>44</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>1</v>
@@ -2227,7 +2237,7 @@
         <v>43</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -2235,28 +2245,28 @@
         <v>2</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -2264,13 +2274,13 @@
         <v>47</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>1</v>
@@ -2279,7 +2289,7 @@
         <v>48</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -2287,22 +2297,22 @@
         <v>49</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>50</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -2310,13 +2320,13 @@
         <v>51</v>
       </c>
       <c r="C39" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="F39" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>1</v>
@@ -2325,7 +2335,7 @@
         <v>52</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -2333,160 +2343,160 @@
         <v>53</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>54</v>
+        <v>185</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>126</v>
+        <v>186</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>169</v>
+        <v>1</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>168</v>
+        <v>187</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="B41" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C41" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="F41" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="B42" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>87</v>
+        <v>185</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>54</v>
+        <v>184</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>126</v>
+        <v>186</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>169</v>
+        <v>1</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>168</v>
+        <v>187</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="B43" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="D43" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="B44" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="B45" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D45" s="3" t="s">
+      <c r="F45" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H45" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F45" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="I45" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="B46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H46" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="I46" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -2494,22 +2504,22 @@
         <v>45</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D47" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="F47" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="G47" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -2517,22 +2527,22 @@
         <v>45</v>
       </c>
       <c r="C48" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="F48" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="F48" s="3" t="s">
-        <v>153</v>
-      </c>
       <c r="G48" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="2:9">
@@ -2540,22 +2550,22 @@
         <v>46</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D49" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F49" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="F49" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="G49" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="2:9">
@@ -2563,22 +2573,22 @@
         <v>46</v>
       </c>
       <c r="C50" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="F50" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="F50" s="3" t="s">
-        <v>153</v>
-      </c>
       <c r="G50" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added price/prt, part amounts and total prices
</commit_message>
<xml_diff>
--- a/docs/low-gain-radio_BOM.xlsx
+++ b/docs/low-gain-radio_BOM.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TheBear\oresat\low-gain-radio\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Oresat\low-gain-radio\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="low-gain-radio_BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="191">
   <si>
     <t>MFG</t>
   </si>
@@ -177,9 +177,6 @@
     <t>U3</t>
   </si>
   <si>
-    <t>W25Q80DVSSIG-ND</t>
-  </si>
-  <si>
     <t>U4</t>
   </si>
   <si>
@@ -583,12 +580,27 @@
   </si>
   <si>
     <t>296-38557-1-ND</t>
+  </si>
+  <si>
+    <t>Price/prt</t>
+  </si>
+  <si>
+    <t>W25Q80DVSNIG-ND</t>
+  </si>
+  <si>
+    <t>Part Amounts</t>
+  </si>
+  <si>
+    <t>Total Price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="21">
     <font>
       <sz val="11"/>
@@ -1040,7 +1052,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1084,8 +1096,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1094,8 +1107,9 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="43" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1123,6 +1137,7 @@
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Currency" xfId="43" builtinId="4"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -1450,10 +1465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1466,12 +1481,16 @@
     <col min="6" max="6" width="82" style="3" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" style="3" customWidth="1"/>
     <col min="8" max="8" width="25.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="3"/>
+    <col min="9" max="9" width="9.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="3"/>
+    <col min="11" max="11" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1481,7 +1500,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:12">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1491,9 +1510,9 @@
       <c r="G2" s="2"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4"/>
@@ -1503,9 +1522,9 @@
       <c r="G3" s="2"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:12">
       <c r="A4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="4"/>
@@ -1515,9 +1534,9 @@
       <c r="G4" s="2"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1527,73 +1546,82 @@
       <c r="G5" s="2"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:12">
       <c r="A6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:12">
       <c r="A7" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:12">
       <c r="A9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="3">
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>2</v>
@@ -1602,24 +1630,34 @@
         <v>3</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="K10" s="3">
+        <v>50</v>
+      </c>
+      <c r="L10" s="6">
+        <f>J10*K10</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="3">
         <v>2</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>2</v>
@@ -1628,24 +1666,34 @@
         <v>4</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J11" s="6">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="K11" s="3">
+        <v>10</v>
+      </c>
+      <c r="L11" s="6">
+        <f t="shared" ref="L11:L50" si="0">J11*K11</f>
+        <v>0.41000000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="3">
         <v>4</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>2</v>
@@ -1654,24 +1702,34 @@
         <v>5</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J12" s="6">
+        <v>2.2200000000000001E-2</v>
+      </c>
+      <c r="K12" s="3">
+        <v>50</v>
+      </c>
+      <c r="L12" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="3">
         <v>4</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>2</v>
@@ -1680,24 +1738,34 @@
         <v>6</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J13" s="6">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="K13" s="3">
+        <v>10</v>
+      </c>
+      <c r="L13" s="6">
+        <f t="shared" si="0"/>
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="3">
         <v>2</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>7</v>
@@ -1706,24 +1774,34 @@
         <v>8</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J14" s="6">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="K14" s="3">
+        <v>50</v>
+      </c>
+      <c r="L14" s="6">
+        <f t="shared" si="0"/>
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="3">
         <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>2</v>
@@ -1732,24 +1810,34 @@
         <v>9</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J15" s="6">
+        <v>6.0400000000000002E-2</v>
+      </c>
+      <c r="K15" s="3">
+        <v>50</v>
+      </c>
+      <c r="L15" s="6">
+        <f t="shared" si="0"/>
+        <v>3.02</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="3">
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>7</v>
@@ -1758,7 +1846,7 @@
         <v>11</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>1</v>
@@ -1767,15 +1855,25 @@
         <v>10</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J16" s="6">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="K16" s="3">
+        <v>100</v>
+      </c>
+      <c r="L16" s="6">
+        <f t="shared" si="0"/>
+        <v>2.1999999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="3">
         <v>3</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>2</v>
@@ -1784,7 +1882,7 @@
         <v>14</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>12</v>
@@ -1793,41 +1891,61 @@
         <v>13</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J17" s="6">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="K17" s="3">
+        <v>50</v>
+      </c>
+      <c r="L17" s="6">
+        <f t="shared" si="0"/>
+        <v>0.27999999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="3">
         <v>2</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>167</v>
-      </c>
       <c r="I18" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J18" s="6">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="K18" s="3">
+        <v>10</v>
+      </c>
+      <c r="L18" s="6">
+        <f t="shared" si="0"/>
+        <v>5.23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="3">
         <v>2</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>2</v>
@@ -1836,19 +1954,29 @@
         <v>15</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J19" s="6">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="K19" s="3">
+        <v>10</v>
+      </c>
+      <c r="L19" s="6">
+        <f t="shared" si="0"/>
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="B20" s="3" t="s">
         <v>16</v>
       </c>
@@ -1859,7 +1987,7 @@
         <v>18</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>1</v>
@@ -1868,10 +1996,20 @@
         <v>17</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J20" s="6">
+        <v>1.25</v>
+      </c>
+      <c r="K20" s="3">
+        <v>5</v>
+      </c>
+      <c r="L20" s="6">
+        <f t="shared" si="0"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
@@ -1882,7 +2020,7 @@
         <v>21</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>12</v>
@@ -1891,15 +2029,25 @@
         <v>20</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J21" s="6">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="K21" s="3">
+        <v>50</v>
+      </c>
+      <c r="L21" s="6">
+        <f t="shared" si="0"/>
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="3">
         <v>3</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>2</v>
@@ -1908,7 +2056,7 @@
         <v>14</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>12</v>
@@ -1917,56 +2065,86 @@
         <v>13</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J22" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="K22" s="3">
+        <v>10</v>
+      </c>
+      <c r="L22" s="6">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="B23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+        <v>144</v>
+      </c>
+      <c r="J23" s="6">
+        <v>5.73</v>
+      </c>
+      <c r="K23" s="3">
+        <v>4</v>
+      </c>
+      <c r="L23" s="6">
+        <f t="shared" si="0"/>
+        <v>22.92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="B24" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>136</v>
-      </c>
       <c r="F24" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <v>144</v>
+      </c>
+      <c r="J24" s="6">
+        <v>3.55</v>
+      </c>
+      <c r="K24" s="3">
+        <v>4</v>
+      </c>
+      <c r="L24" s="6">
+        <f t="shared" si="0"/>
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="B25" s="3" t="s">
         <v>24</v>
       </c>
@@ -1977,7 +2155,7 @@
         <v>27</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>12</v>
@@ -1986,29 +2164,49 @@
         <v>25</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J25" s="6">
+        <v>0.45</v>
+      </c>
+      <c r="K25" s="3">
+        <v>10</v>
+      </c>
+      <c r="L25" s="6">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="B26" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>142</v>
-      </c>
       <c r="I26" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J26" s="6">
+        <v>0.45</v>
+      </c>
+      <c r="K26" s="3">
+        <v>5</v>
+      </c>
+      <c r="L26" s="6">
+        <f t="shared" si="0"/>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" s="3">
         <v>2</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>2</v>
@@ -2017,7 +2215,7 @@
         <v>29</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>1</v>
@@ -2026,15 +2224,25 @@
         <v>28</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J27" s="6">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="K27" s="3">
+        <v>10</v>
+      </c>
+      <c r="L27" s="6">
+        <f t="shared" si="0"/>
+        <v>1.6500000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="3">
         <v>4</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>2</v>
@@ -2043,7 +2251,7 @@
         <v>31</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>1</v>
@@ -2052,10 +2260,20 @@
         <v>30</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J28" s="6">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="K28" s="3">
+        <v>10</v>
+      </c>
+      <c r="L28" s="6">
+        <f t="shared" si="0"/>
+        <v>1.6500000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="B29" s="3" t="s">
         <v>32</v>
       </c>
@@ -2066,24 +2284,34 @@
         <v>33</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J29" s="6">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="K29" s="3">
+        <v>10</v>
+      </c>
+      <c r="L29" s="6">
+        <f t="shared" si="0"/>
+        <v>1.6500000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="3">
         <v>4</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>35</v>
@@ -2092,10 +2320,10 @@
         <v>36</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>1</v>
@@ -2104,39 +2332,59 @@
         <v>34</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J30" s="6">
+        <v>0.222</v>
+      </c>
+      <c r="K30" s="3">
+        <v>10</v>
+      </c>
+      <c r="L30" s="6">
+        <f t="shared" si="0"/>
+        <v>2.2200000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="3">
         <v>4</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>170</v>
-      </c>
       <c r="E31" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J31" s="6">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="6">
+        <f t="shared" si="0"/>
+        <v>4.8599999999999994</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="B32" s="3" t="s">
         <v>37</v>
       </c>
@@ -2147,24 +2395,34 @@
         <v>39</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J32" s="6">
+        <v>1.4E-2</v>
+      </c>
+      <c r="K32" s="3">
+        <v>10</v>
+      </c>
+      <c r="L32" s="6">
+        <f t="shared" si="0"/>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="3">
         <v>3</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>41</v>
@@ -2173,7 +2431,7 @@
         <v>42</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>1</v>
@@ -2182,15 +2440,25 @@
         <v>40</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J33" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="K33" s="3">
+        <v>25</v>
+      </c>
+      <c r="L33" s="6">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" s="3">
         <v>6</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>41</v>
@@ -2199,7 +2467,7 @@
         <v>44</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>1</v>
@@ -2208,15 +2476,25 @@
         <v>43</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J34" s="6">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="K34" s="3">
+        <v>50</v>
+      </c>
+      <c r="L34" s="6">
+        <f t="shared" si="0"/>
+        <v>0.28500000000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" s="3">
         <v>2</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>41</v>
@@ -2225,10 +2503,10 @@
         <v>44</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>1</v>
@@ -2237,50 +2515,70 @@
         <v>43</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J35" s="6">
+        <v>1.4E-2</v>
+      </c>
+      <c r="K35" s="3">
+        <v>100</v>
+      </c>
+      <c r="L35" s="6">
+        <f t="shared" si="0"/>
+        <v>1.4000000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" s="3">
         <v>2</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="J36" s="6">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="K36" s="3">
+        <v>10</v>
+      </c>
+      <c r="L36" s="6">
+        <f t="shared" si="0"/>
+        <v>0.10999999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="B37" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>1</v>
@@ -2289,306 +2587,452 @@
         <v>48</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+        <v>144</v>
+      </c>
+      <c r="J37" s="6">
+        <v>4.34</v>
+      </c>
+      <c r="K37" s="3">
+        <v>4</v>
+      </c>
+      <c r="L37" s="6">
+        <f t="shared" si="0"/>
+        <v>17.36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="B38" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>50</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
+        <v>144</v>
+      </c>
+      <c r="J38" s="6">
+        <v>5.99</v>
+      </c>
+      <c r="K38" s="3">
+        <v>4</v>
+      </c>
+      <c r="L38" s="6">
+        <f t="shared" si="0"/>
+        <v>23.96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="B39" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C39" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="F39" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J39" s="6">
+        <v>0.36</v>
+      </c>
+      <c r="K39" s="3">
+        <v>4</v>
+      </c>
+      <c r="L39" s="6">
+        <f t="shared" si="0"/>
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="B40" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J40" s="6">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="K40" s="3">
+        <v>5</v>
+      </c>
+      <c r="L40" s="6">
+        <f t="shared" si="0"/>
+        <v>2.8499999999999996</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="B41" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F39" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="B40" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C40" s="3" t="s">
+      <c r="D41" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J41" s="6">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="K41" s="3">
+        <v>10</v>
+      </c>
+      <c r="L41" s="6">
+        <f t="shared" si="0"/>
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="B42" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="F40" s="3" t="s">
+      <c r="G42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H42" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="G40" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I40" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="B41" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D41" s="3" t="s">
+      <c r="I42" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J42" s="6">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="K42" s="3">
+        <v>5</v>
+      </c>
+      <c r="L42" s="6">
+        <f t="shared" si="0"/>
+        <v>2.8499999999999996</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="B43" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J43" s="6">
+        <v>1.52</v>
+      </c>
+      <c r="K43" s="3">
+        <v>4</v>
+      </c>
+      <c r="L43" s="6">
+        <f t="shared" si="0"/>
+        <v>6.08</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="B44" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="J44" s="6">
+        <v>3</v>
+      </c>
+      <c r="K44" s="3">
+        <v>4</v>
+      </c>
+      <c r="L44" s="6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="B45" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F41" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="B42" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I42" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="B43" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="F43" s="3" t="s">
+      <c r="D45" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="J45" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="K45" s="3">
+        <v>4</v>
+      </c>
+      <c r="L45" s="6">
+        <f t="shared" si="0"/>
+        <v>3.32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="B46" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F46" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="G43" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="B44" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="I44" s="3" t="s">
+      <c r="G46" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I46" s="3" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="B45" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I45" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="B46" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="J46" s="6">
+        <v>0.82</v>
+      </c>
+      <c r="K46" s="3">
+        <v>4</v>
+      </c>
+      <c r="L46" s="6">
+        <f t="shared" si="0"/>
+        <v>3.28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="B47" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F47" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H47" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="G47" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>153</v>
-      </c>
       <c r="I47" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
+        <v>144</v>
+      </c>
+      <c r="J47" s="6">
+        <v>1.2869999999999999</v>
+      </c>
+      <c r="K47" s="3">
+        <v>5</v>
+      </c>
+      <c r="L47" s="6">
+        <f t="shared" si="0"/>
+        <v>6.4349999999999996</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="B48" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C48" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H48" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>148</v>
-      </c>
       <c r="I48" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="49" spans="2:9">
+        <v>144</v>
+      </c>
+      <c r="J48" s="6">
+        <v>1.6579999999999999</v>
+      </c>
+      <c r="K48" s="3">
+        <v>5</v>
+      </c>
+      <c r="L48" s="6">
+        <f t="shared" si="0"/>
+        <v>8.2899999999999991</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12">
       <c r="B49" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F49" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H49" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="G49" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>153</v>
-      </c>
       <c r="I49" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9">
+        <v>144</v>
+      </c>
+      <c r="J49" s="6">
+        <v>1.2869999999999999</v>
+      </c>
+      <c r="K49" s="3">
+        <v>5</v>
+      </c>
+      <c r="L49" s="6">
+        <f t="shared" si="0"/>
+        <v>6.4349999999999996</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12">
       <c r="B50" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C50" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H50" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>148</v>
-      </c>
       <c r="I50" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
+      </c>
+      <c r="J50" s="6">
+        <v>1.6579999999999999</v>
+      </c>
+      <c r="K50" s="3">
+        <v>5</v>
+      </c>
+      <c r="L50" s="6">
+        <f t="shared" si="0"/>
+        <v>8.2899999999999991</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12">
+      <c r="L51" s="6">
+        <f>SUM(L10:L50)</f>
+        <v>200.88500000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced SkyWorks switch on BOM with Peregrine one
</commit_message>
<xml_diff>
--- a/docs/low-gain-radio_BOM.xlsx
+++ b/docs/low-gain-radio_BOM.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Oresat\low-gain-radio\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TheBear\oresat\low-gain-radio\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="low-gain-radio_BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="192">
   <si>
     <t>MFG</t>
   </si>
@@ -198,12 +198,6 @@
     <t>U9</t>
   </si>
   <si>
-    <t>SKY13405-490LF</t>
-  </si>
-  <si>
-    <t>863-1649-1-ND</t>
-  </si>
-  <si>
     <t>Y1</t>
   </si>
   <si>
@@ -402,9 +396,6 @@
     <t>Crystals 32MHz 10ppm 12pF -30C +85C</t>
   </si>
   <si>
-    <t>RF Switch ICs .01-3GHz SP2T UHL Switch</t>
-  </si>
-  <si>
     <t>IC FLASH 8MBIT 104MHZ 8SOIC</t>
   </si>
   <si>
@@ -592,12 +583,24 @@
   </si>
   <si>
     <t>Total Price</t>
+  </si>
+  <si>
+    <t>Peregrine Semiconductor</t>
+  </si>
+  <si>
+    <t>PE42723A-Z</t>
+  </si>
+  <si>
+    <t>UltraCMOS® SPDT RF Switch, 5–1794 MHz</t>
+  </si>
+  <si>
+    <t>1046-1150-1-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -1465,32 +1468,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="33.875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="24.625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="24.25" style="3" customWidth="1"/>
+    <col min="5" max="5" width="6.875" style="3" customWidth="1"/>
     <col min="6" max="6" width="82" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="25.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="3"/>
-    <col min="11" max="11" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="3"/>
+    <col min="7" max="7" width="10.875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="25.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.125" style="3"/>
+    <col min="11" max="11" width="13.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1512,7 +1515,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4"/>
@@ -1524,7 +1527,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="4"/>
@@ -1536,7 +1539,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1548,14 +1551,14 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -1564,14 +1567,14 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1580,40 +1583,40 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J9" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="L9" s="3" t="s">
         <v>187</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1621,7 +1624,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>2</v>
@@ -1630,16 +1633,16 @@
         <v>3</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J10" s="6">
         <v>0.01</v>
@@ -1657,7 +1660,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>2</v>
@@ -1666,16 +1669,16 @@
         <v>4</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J11" s="6">
         <v>4.1000000000000002E-2</v>
@@ -1693,7 +1696,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>2</v>
@@ -1702,16 +1705,16 @@
         <v>5</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J12" s="6">
         <v>2.2200000000000001E-2</v>
@@ -1729,7 +1732,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>2</v>
@@ -1738,16 +1741,16 @@
         <v>6</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J13" s="6">
         <v>5.2999999999999999E-2</v>
@@ -1765,7 +1768,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>7</v>
@@ -1774,16 +1777,16 @@
         <v>8</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J14" s="6">
         <v>0.34200000000000003</v>
@@ -1801,7 +1804,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>2</v>
@@ -1810,16 +1813,16 @@
         <v>9</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J15" s="6">
         <v>6.0400000000000002E-2</v>
@@ -1837,7 +1840,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>7</v>
@@ -1846,7 +1849,7 @@
         <v>11</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>1</v>
@@ -1855,7 +1858,7 @@
         <v>10</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J16" s="6">
         <v>2.1999999999999999E-2</v>
@@ -1873,7 +1876,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>2</v>
@@ -1882,7 +1885,7 @@
         <v>14</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>12</v>
@@ -1891,7 +1894,7 @@
         <v>13</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J17" s="6">
         <v>5.5999999999999999E-3</v>
@@ -1909,25 +1912,25 @@
         <v>2</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J18" s="6">
         <v>0.52300000000000002</v>
@@ -1945,7 +1948,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>2</v>
@@ -1954,16 +1957,16 @@
         <v>15</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J19" s="6">
         <v>3.5999999999999997E-2</v>
@@ -1987,7 +1990,7 @@
         <v>18</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>1</v>
@@ -1996,7 +1999,7 @@
         <v>17</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J20" s="6">
         <v>1.25</v>
@@ -2020,7 +2023,7 @@
         <v>21</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>12</v>
@@ -2029,7 +2032,7 @@
         <v>20</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J21" s="6">
         <v>5.1999999999999998E-3</v>
@@ -2047,7 +2050,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>2</v>
@@ -2056,7 +2059,7 @@
         <v>14</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>12</v>
@@ -2065,7 +2068,7 @@
         <v>13</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J22" s="6">
         <v>0.01</v>
@@ -2083,22 +2086,22 @@
         <v>22</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J23" s="6">
         <v>5.73</v>
@@ -2116,22 +2119,22 @@
         <v>23</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>137</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J24" s="6">
         <v>3.55</v>
@@ -2155,7 +2158,7 @@
         <v>27</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>12</v>
@@ -2164,7 +2167,7 @@
         <v>25</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J25" s="6">
         <v>0.45</v>
@@ -2179,16 +2182,16 @@
     </row>
     <row r="26" spans="1:12">
       <c r="B26" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J26" s="6">
         <v>0.45</v>
@@ -2206,7 +2209,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>2</v>
@@ -2215,7 +2218,7 @@
         <v>29</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>1</v>
@@ -2224,7 +2227,7 @@
         <v>28</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J27" s="6">
         <v>0.16500000000000001</v>
@@ -2242,7 +2245,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>2</v>
@@ -2251,7 +2254,7 @@
         <v>31</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>1</v>
@@ -2260,7 +2263,7 @@
         <v>30</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J28" s="6">
         <v>0.16500000000000001</v>
@@ -2284,16 +2287,16 @@
         <v>33</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J29" s="6">
         <v>0.16500000000000001</v>
@@ -2311,7 +2314,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>35</v>
@@ -2320,10 +2323,10 @@
         <v>36</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>1</v>
@@ -2332,7 +2335,7 @@
         <v>34</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J30" s="6">
         <v>0.222</v>
@@ -2350,28 +2353,28 @@
         <v>4</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J31" s="6">
         <v>0.48599999999999999</v>
@@ -2395,16 +2398,16 @@
         <v>39</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J32" s="6">
         <v>1.4E-2</v>
@@ -2422,7 +2425,7 @@
         <v>3</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>41</v>
@@ -2431,7 +2434,7 @@
         <v>42</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>1</v>
@@ -2440,7 +2443,7 @@
         <v>40</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J33" s="6">
         <v>0.01</v>
@@ -2458,7 +2461,7 @@
         <v>6</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>41</v>
@@ -2467,7 +2470,7 @@
         <v>44</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>1</v>
@@ -2476,7 +2479,7 @@
         <v>43</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J34" s="6">
         <v>5.7000000000000002E-3</v>
@@ -2494,7 +2497,7 @@
         <v>2</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>41</v>
@@ -2503,10 +2506,10 @@
         <v>44</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>1</v>
@@ -2515,7 +2518,7 @@
         <v>43</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J35" s="6">
         <v>1.4E-2</v>
@@ -2533,28 +2536,28 @@
         <v>2</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D36" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="G36" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J36" s="6">
         <v>1.0999999999999999E-2</v>
@@ -2572,13 +2575,13 @@
         <v>47</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>1</v>
@@ -2587,7 +2590,7 @@
         <v>48</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J37" s="6">
         <v>4.34</v>
@@ -2605,22 +2608,22 @@
         <v>49</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>50</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J38" s="6">
         <v>5.99</v>
@@ -2638,22 +2641,22 @@
         <v>51</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J39" s="6">
         <v>0.36</v>
@@ -2671,22 +2674,22 @@
         <v>52</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D40" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H40" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="F40" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>186</v>
-      </c>
       <c r="I40" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J40" s="6">
         <v>0.56999999999999995</v>
@@ -2704,22 +2707,22 @@
         <v>53</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J41" s="6">
         <v>0.28599999999999998</v>
@@ -2737,22 +2740,22 @@
         <v>54</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D42" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H42" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="F42" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>186</v>
-      </c>
       <c r="I42" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J42" s="6">
         <v>0.56999999999999995</v>
@@ -2773,19 +2776,19 @@
         <v>56</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J43" s="6">
         <v>1.52</v>
@@ -2803,22 +2806,22 @@
         <v>57</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J44" s="6">
         <v>3</v>
@@ -2836,55 +2839,55 @@
         <v>58</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>85</v>
+        <v>188</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>127</v>
+        <v>189</v>
+      </c>
+      <c r="F45" t="s">
+        <v>190</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>60</v>
+        <v>191</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J45" s="6">
-        <v>0.83</v>
+        <v>4.59</v>
       </c>
       <c r="K45" s="3">
         <v>4</v>
       </c>
       <c r="L45" s="6">
         <f t="shared" si="0"/>
-        <v>3.32</v>
+        <v>18.36</v>
       </c>
     </row>
     <row r="46" spans="1:12">
       <c r="B46" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J46" s="6">
         <v>0.82</v>
@@ -2902,22 +2905,22 @@
         <v>45</v>
       </c>
       <c r="C47" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="F47" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H47" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="F47" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I47" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J47" s="6">
         <v>1.2869999999999999</v>
@@ -2935,22 +2938,22 @@
         <v>45</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J48" s="6">
         <v>1.6579999999999999</v>
@@ -2968,22 +2971,22 @@
         <v>46</v>
       </c>
       <c r="C49" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="F49" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H49" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="F49" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I49" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J49" s="6">
         <v>1.2869999999999999</v>
@@ -3001,22 +3004,22 @@
         <v>46</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J50" s="6">
         <v>1.6579999999999999</v>
@@ -3030,9 +3033,13 @@
       </c>
     </row>
     <row r="51" spans="2:12">
-      <c r="L51" s="6">
+      <c r="J51" s="6"/>
+      <c r="L51" s="6"/>
+    </row>
+    <row r="52" spans="2:12">
+      <c r="L52" s="6">
         <f>SUM(L10:L50)</f>
-        <v>200.88500000000002</v>
+        <v>215.92500000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>